<commit_message>
scene totals for categories
</commit_message>
<xml_diff>
--- a/xlsx/subcategory_scene_counts.xlsx
+++ b/xlsx/subcategory_scene_counts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\A\Grad_School\Uwyo\assistantships\research\grocery\nerfbaselines-grocery\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA02480-DAB6-4055-86DF-224589CC8B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D8038C-F4DF-4B8F-A3D7-8FB6B5EEF3BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28920" yWindow="2460" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="80">
   <si>
     <t>Apples</t>
   </si>
@@ -263,13 +263,19 @@
     <t>VariousVeggies</t>
   </si>
   <si>
-    <t>overall</t>
-  </si>
-  <si>
     <t>scene</t>
   </si>
   <si>
     <t>amount</t>
+  </si>
+  <si>
+    <t>sum</t>
+  </si>
+  <si>
+    <t>sum overall</t>
+  </si>
+  <si>
+    <t>avg overall</t>
   </si>
 </sst>
 </file>
@@ -279,8 +285,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -308,9 +324,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,10 +608,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B85"/>
+  <dimension ref="A1:B89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,12 +620,12 @@
     <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="B1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -731,82 +749,83 @@
       </c>
     </row>
     <row r="17" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18">
+        <f>SUM(B2:B16)</f>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B19" s="1">
         <f>AVERAGE(B2:B16)</f>
         <v>9.6</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20">
-        <v>2</v>
-      </c>
-    </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B21">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B22">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B23">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B24">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B25">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B26">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B27">
-        <v>17</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B28">
         <v>17</v>
@@ -814,15 +833,15 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B29">
-        <v>2</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -830,79 +849,79 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B31">
-        <v>34</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B32">
-        <v>2</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B33">
-        <v>18</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B34">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B35">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B36">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B37">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B38">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B39">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B40">
         <v>3</v>
@@ -910,143 +929,143 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B41">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B42">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B43">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B44">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B45">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B46">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B47">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B48">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B49">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B50">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B51">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B52">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B53">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B54">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B55">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B56">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B57">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B58">
         <v>4</v>
@@ -1054,188 +1073,223 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B59">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B60">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B61">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B62">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B63">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B64">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>59</v>
+      </c>
+      <c r="B65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>60</v>
       </c>
-      <c r="B65">
+      <c r="B66">
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>61</v>
-      </c>
-      <c r="B67" s="1">
-        <f>AVERAGE(B20:B65)</f>
-        <v>6.6521739130434785</v>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>77</v>
+      </c>
+      <c r="B68">
+        <f>SUM(B21:B66)</f>
+        <v>306</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>62</v>
-      </c>
-      <c r="B69">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>63</v>
-      </c>
-      <c r="B70">
-        <v>2</v>
+        <v>61</v>
+      </c>
+      <c r="B69" s="1">
+        <f>AVERAGE(B21:B66)</f>
+        <v>6.6521739130434785</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B71">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B72">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B73">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B74">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B75">
-        <v>21</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B76">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B77">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B78">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B79">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B80">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B81">
-        <v>7</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>73</v>
+      </c>
+      <c r="B82">
+        <v>16</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>61</v>
-      </c>
-      <c r="B83" s="1">
-        <f>AVERAGE(B69:B81)</f>
-        <v>7.4615384615384617</v>
+        <v>74</v>
+      </c>
+      <c r="B83">
+        <v>7</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>75</v>
-      </c>
-      <c r="B85" s="1">
-        <f>AVERAGE(B2:B16,B20:B65,B69:B81)</f>
+        <v>77</v>
+      </c>
+      <c r="B85">
+        <f>SUM(B71:B83)</f>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>61</v>
+      </c>
+      <c r="B86" s="1">
+        <f>AVERAGE(B71:B83)</f>
+        <v>7.4615384615384617</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>78</v>
+      </c>
+      <c r="B88">
+        <f>SUM(B21:B66,B71:B83,B2:B16)</f>
+        <v>547</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>79</v>
+      </c>
+      <c r="B89" s="1">
+        <f>AVERAGE(B2:B16,B21:B66,B71:B83)</f>
         <v>7.3918918918918921</v>
       </c>
     </row>

</xml_diff>